<commit_message>
rebase on openurp 0.30.x
</commit_message>
<xml_diff>
--- a/audit/src/main/resources/org/openurp/std/graduation/degree/degree_apply.xlsx
+++ b/audit/src/main/resources/org/openurp/std/graduation/degree/degree_apply.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7270"/>
+    <workbookView windowWidth="20490" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,10 +160,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -199,14 +199,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,36 +243,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -289,10 +281,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -304,13 +297,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -327,6 +313,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +329,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -356,187 +356,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,15 +647,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,8 +684,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,6 +731,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -756,10 +756,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -768,33 +768,36 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -804,97 +807,94 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1298,24 +1298,24 @@
   <sheetPr/>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.4545454545455" customWidth="1"/>
-    <col min="2" max="2" width="5.36363636363636" customWidth="1"/>
+    <col min="1" max="1" width="10.4583333333333" customWidth="1"/>
+    <col min="2" max="2" width="5.36666666666667" customWidth="1"/>
     <col min="3" max="3" width="3" customWidth="1"/>
-    <col min="6" max="6" width="3.90909090909091" customWidth="1"/>
-    <col min="7" max="7" width="2.90909090909091" customWidth="1"/>
-    <col min="8" max="8" width="17.0909090909091" customWidth="1"/>
-    <col min="9" max="9" width="2.36363636363636" customWidth="1"/>
-    <col min="10" max="10" width="10.3636363636364" customWidth="1"/>
-    <col min="11" max="11" width="20.7272727272727" customWidth="1"/>
+    <col min="6" max="6" width="3.90833333333333" customWidth="1"/>
+    <col min="7" max="7" width="2.90833333333333" customWidth="1"/>
+    <col min="8" max="8" width="17.0916666666667" customWidth="1"/>
+    <col min="9" max="9" width="2.36666666666667" customWidth="1"/>
+    <col min="10" max="10" width="10.3666666666667" customWidth="1"/>
+    <col min="11" max="11" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="29" spans="1:11">
+    <row r="1" ht="28.5" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" ht="106" customHeight="1" spans="1:11">
+    <row r="7" ht="95" customHeight="1" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" ht="125" customHeight="1" spans="1:11">
+    <row r="10" ht="109" customHeight="1" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="J12" s="12"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" ht="120" customHeight="1" spans="1:11">
+    <row r="13" ht="108" customHeight="1" spans="1:11">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
update to api 0.32.2
</commit_message>
<xml_diff>
--- a/audit/src/main/resources/org/openurp/std/graduation/degree/degree_apply.xlsx
+++ b/audit/src/main/resources/org/openurp/std/graduation/degree/degree_apply.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7860"/>
+    <workbookView windowWidth="30720" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>${school}学士学位申请表</t>
   </si>
@@ -119,9 +119,6 @@
   <si>
     <t>学院
 审查意见</t>
-  </si>
-  <si>
-    <t>　　　　　　　　　　院长：签名（盖章）</t>
   </si>
   <si>
     <t>20 　年　　月　　日</t>
@@ -1299,23 +1296,23 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:K19"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.72222222222222" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.4583333333333" customWidth="1"/>
-    <col min="2" max="2" width="5.36666666666667" customWidth="1"/>
+    <col min="1" max="1" width="10.4537037037037" customWidth="1"/>
+    <col min="2" max="2" width="5.37037037037037" customWidth="1"/>
     <col min="3" max="3" width="3" customWidth="1"/>
-    <col min="6" max="6" width="3.90833333333333" customWidth="1"/>
-    <col min="7" max="7" width="2.90833333333333" customWidth="1"/>
-    <col min="8" max="8" width="17.0916666666667" customWidth="1"/>
-    <col min="9" max="9" width="2.36666666666667" customWidth="1"/>
-    <col min="10" max="10" width="10.3666666666667" customWidth="1"/>
-    <col min="11" max="11" width="19.875" customWidth="1"/>
+    <col min="6" max="6" width="3.90740740740741" customWidth="1"/>
+    <col min="7" max="7" width="2.90740740740741" customWidth="1"/>
+    <col min="8" max="8" width="17.0925925925926" customWidth="1"/>
+    <col min="9" max="9" width="2.37037037037037" customWidth="1"/>
+    <col min="10" max="10" width="10.3703703703704" customWidth="1"/>
+    <col min="11" max="11" width="19.8796296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28.5" spans="1:11">
+    <row r="1" ht="29.4" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1450,11 +1447,9 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" ht="14.15" customHeight="1" spans="1:11">
+    <row r="8" ht="14.15" hidden="1" customHeight="1" spans="1:11">
       <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1468,7 +1463,7 @@
     <row r="9" ht="14.15" customHeight="1" spans="1:11">
       <c r="A9" s="8"/>
       <c r="B9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1482,7 +1477,7 @@
     </row>
     <row r="10" ht="109" customHeight="1" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1498,7 +1493,7 @@
     <row r="11" ht="14.15" customHeight="1" spans="1:11">
       <c r="A11" s="8"/>
       <c r="B11" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1525,7 +1520,7 @@
     </row>
     <row r="13" ht="108" customHeight="1" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1541,7 +1536,7 @@
     <row r="14" ht="14.15" customHeight="1" spans="1:11">
       <c r="A14" s="8"/>
       <c r="B14" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1568,10 +1563,10 @@
     </row>
     <row r="16" ht="22.65" customHeight="1" spans="1:11">
       <c r="A16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -1586,7 +1581,7 @@
     <row r="17" ht="22.65" customHeight="1" spans="1:11">
       <c r="A17" s="8"/>
       <c r="B17" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -1601,7 +1596,7 @@
     <row r="18" ht="22.65" customHeight="1" spans="1:11">
       <c r="A18" s="8"/>
       <c r="B18" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -1615,7 +1610,7 @@
     </row>
     <row r="19" ht="112" customHeight="1" spans="1:11">
       <c r="A19" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>

</xml_diff>